<commit_message>
minor fix; more tests;
</commit_message>
<xml_diff>
--- a/demo/files/demo-02-advanced.xlsx
+++ b/demo/files/demo-02-advanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72595E7B-41C9-4BC7-8995-766221447C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105F4AF1-77E7-4E6C-9883-A5E55EDED98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="63855" yWindow="2415" windowWidth="18510" windowHeight="11565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Lorem</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Data of Sheet2 (part 2)</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -284,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -294,8 +297,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -308,10 +309,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -603,11 +607,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="1" t="s">
@@ -711,232 +715,236 @@
   <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="F2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>2000</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>235</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="11">
         <v>81.955861416002492</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>2009</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>433</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <v>333.14716577166655</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <f>B5+1</f>
         <v>2001</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>859</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>64.137997890820259</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <f>F5+1</f>
         <v>2010</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>365</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <v>361.04943821518521</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <f t="shared" ref="B7:B13" si="0">B6+1</f>
         <v>2002</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>642</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>180.71226210095296</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <f t="shared" ref="F7:F13" si="1">F6+1</f>
         <v>2011</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="9">
         <v>705</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <v>684.10559098745489</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <f t="shared" si="0"/>
         <v>2003</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>780</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>447.57921566992451</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <f t="shared" si="1"/>
         <v>2012</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <v>236</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <v>75.788099017385562</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <f t="shared" si="0"/>
         <v>2004</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>769</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>300.04310032896188</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>2013</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="9">
         <v>107</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>25.216493632314481</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>682</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>163.2379099256749</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <f t="shared" si="1"/>
         <v>2014</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <v>523</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="12">
         <v>407.96178422724222</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <f t="shared" si="0"/>
         <v>2006</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>392</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>304.7729077428578</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <f t="shared" si="1"/>
         <v>2015</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="9">
         <v>503</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="12">
         <v>59.432700113871611</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <f t="shared" si="0"/>
         <v>2007</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="9">
         <v>216</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>120.17578666694905</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="9">
         <v>810</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="12">
         <v>560.80667691479698</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <f t="shared" si="0"/>
         <v>2008</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="10">
         <v>674</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="13">
         <v>103.62108685759928</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <f t="shared" si="1"/>
         <v>2017</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="10">
         <v>334</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="13">
         <v>93.410923396310864</v>
       </c>
     </row>

</xml_diff>

<commit_message>
set read area by defined names
</commit_message>
<xml_diff>
--- a/demo/files/demo-02-advanced.xlsx
+++ b/demo/files/demo-02-advanced.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105F4AF1-77E7-4E6C-9883-A5E55EDED98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA616E99-F1BC-4130-8B22-E333CC10B80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63855" yWindow="2415" windowWidth="18510" windowHeight="11565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59355" yWindow="1755" windowWidth="21600" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo1" sheetId="2" r:id="rId1"/>
     <sheet name="Demo2" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Headers">Demo1!$B$4:$D$4</definedName>
+    <definedName name="Values">Demo1!$B$5:$D$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -306,10 +310,10 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -595,9 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9365D91A-FBDF-4F32-8A11-868EB6F27A61}">
   <dimension ref="B2:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -607,11 +609,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="1" t="s">
@@ -714,41 +716,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="F2" s="14" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="F2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new method in Excel - dateFormatter(); new methods in Sheet - firstRow(), firstCol(), readFirstRow(), readFirstRowWithStyles(); new behavior - force fill rows if setReadArea() or if set Excel::KEYS_FIRST_ROW;
</commit_message>
<xml_diff>
--- a/demo/files/demo-02-advanced.xlsx
+++ b/demo/files/demo-02-advanced.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA616E99-F1BC-4130-8B22-E333CC10B80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72601CBA-2741-4A0B-A595-D5F57B878A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59355" yWindow="1755" windowWidth="21600" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="62115" yWindow="1650" windowWidth="17280" windowHeight="8910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo1" sheetId="2" r:id="rId1"/>
     <sheet name="Demo2" sheetId="1" r:id="rId2"/>
+    <sheet name="Demo3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Headers">Demo1!$B$4:$D$4</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Lorem</t>
   </si>
@@ -107,6 +108,18 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>ddd</t>
   </si>
 </sst>
 </file>
@@ -318,8 +331,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -599,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9365D91A-FBDF-4F32-8A11-868EB6F27A61}">
   <dimension ref="B2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -958,4 +971,69 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5420A4A5-7072-46C3-AD6B-F0C13EE92B8F}">
+  <dimension ref="A2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>333</v>
+      </c>
+      <c r="D3">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix - returns empty cells as an empty string
</commit_message>
<xml_diff>
--- a/demo/files/demo-02-advanced.xlsx
+++ b/demo/files/demo-02-advanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72601CBA-2741-4A0B-A595-D5F57B878A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8679CA75-28AC-49A6-B6E3-F2E9CF7C0A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62115" yWindow="1650" windowWidth="17280" windowHeight="8910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="64515" yWindow="5790" windowWidth="17280" windowHeight="8910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo1" sheetId="2" r:id="rId1"/>

</xml_diff>